<commit_message>
[KPI] data sheets and updates
</commit_message>
<xml_diff>
--- a/bloomreach/datasheets/age.xlsx
+++ b/bloomreach/datasheets/age.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gareth.joyce/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gareth.joyce/Desktop/Projects/03-NHS-D/ARM/ur-nhsd/bloomreach/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60058F54-4DAA-FF4E-9AE9-F979A9189DB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0859578C-6F8D-FF4A-A014-D8382836A85B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2720" windowWidth="23880" windowHeight="17040" xr2:uid="{1C0AD7F5-B4CA-144C-84BC-A59D27122AFC}"/>
+    <workbookView xWindow="-26100" yWindow="1340" windowWidth="23880" windowHeight="17040" xr2:uid="{1C0AD7F5-B4CA-144C-84BC-A59D27122AFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>